<commit_message>
Version 2.2.7 Log para controlar cambios
</commit_message>
<xml_diff>
--- a/Jeic/Jeic/Resources/Plantilla.xlsx
+++ b/Jeic/Jeic/Resources/Plantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\bin\Debug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\boxbu\source\repos\Axdrox\proyectoJeic\Jeic\Jeic\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F5AD2A9-C123-422E-95DE-066AD78111AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17596D62-2C53-43AA-85EC-91080C9368EF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -302,36 +302,48 @@
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="3" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -669,248 +681,250 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:BB9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR1" workbookViewId="0">
-      <selection activeCell="BB8" sqref="BB8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="7.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="7" style="2" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="7.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="28.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="7.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7" style="1" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="21.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="16.109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="16.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="18.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="24" style="3" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="30.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="34.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="36" style="1" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="53" style="1" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="22.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="27.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="8.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="22.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21.88671875" style="13" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="16.109375" style="13" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5546875" style="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="16.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.44140625" style="13" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="24" style="2" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="30.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="34.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="36" style="9" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="53" style="9" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="16.88671875" style="5" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="19" style="5" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="24.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="27.5546875" style="13" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="24.33203125" style="13" bestFit="1" customWidth="1"/>
     <col min="42" max="42" width="16.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="14.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="24.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="24.33203125" style="2" customWidth="1"/>
-    <col min="46" max="47" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="24.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="24.33203125" style="5" customWidth="1"/>
+    <col min="46" max="46" width="23.44140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="48" max="48" width="19.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="22.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="50" max="50" width="18" style="1" bestFit="1" customWidth="1"/>
-    <col min="51" max="52" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="10.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="16.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="55" max="16384" width="8.88671875" style="1"/>
+    <col min="51" max="51" width="15" style="1" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="15" style="5" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="10.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="16.21875" style="5" bestFit="1" customWidth="1"/>
+    <col min="55" max="16384" width="8.88671875" style="5"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="L2" s="9" t="s">
+      <c r="L2" s="6" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="G3" s="11"/>
-      <c r="H3" s="11"/>
-      <c r="I3" s="11"/>
-      <c r="J3" s="11"/>
-      <c r="K3" s="11"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
+      <c r="K3" s="15"/>
     </row>
-    <row r="8" spans="1:54" s="10" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+    <row r="8" spans="1:54" s="9" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="H8" s="4" t="s">
+      <c r="H8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="I8" s="4" t="s">
+      <c r="I8" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="J8" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="K8" s="4" t="s">
+      <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="L8" s="4" t="s">
+      <c r="L8" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="M8" s="4" t="s">
+      <c r="M8" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="N8" s="4" t="s">
+      <c r="N8" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="O8" s="4" t="s">
+      <c r="O8" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="P8" s="4" t="s">
+      <c r="P8" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="Q8" s="5" t="s">
+      <c r="Q8" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="T8" s="4" t="s">
+      <c r="T8" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="U8" s="4" t="s">
+      <c r="U8" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="V8" s="4" t="s">
+      <c r="V8" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="W8" s="4" t="s">
+      <c r="W8" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="X8" s="4" t="s">
+      <c r="X8" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="Y8" s="4" t="s">
+      <c r="Y8" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="Z8" s="4" t="s">
+      <c r="Z8" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="AA8" s="4" t="s">
+      <c r="AA8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="AB8" s="4" t="s">
+      <c r="AB8" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="AC8" s="4" t="s">
+      <c r="AC8" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AD8" s="4" t="s">
+      <c r="AD8" s="14" t="s">
         <v>23</v>
       </c>
-      <c r="AE8" s="4" t="s">
+      <c r="AE8" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="AF8" s="4" t="s">
+      <c r="AF8" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="AG8" s="6" t="s">
+      <c r="AG8" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AH8" s="4" t="s">
+      <c r="AH8" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="AI8" s="4" t="s">
+      <c r="AI8" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="AJ8" s="4" t="s">
+      <c r="AJ8" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="AK8" s="4" t="s">
+      <c r="AK8" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AL8" s="4" t="s">
+      <c r="AL8" s="14" t="s">
         <v>28</v>
       </c>
-      <c r="AM8" s="4" t="s">
+      <c r="AM8" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AN8" s="4" t="s">
+      <c r="AN8" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="AO8" s="4" t="s">
+      <c r="AO8" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="AP8" s="4" t="s">
+      <c r="AP8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="AQ8" s="4" t="s">
+      <c r="AQ8" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="AR8" s="4" t="s">
+      <c r="AR8" s="7" t="s">
         <v>34</v>
       </c>
-      <c r="AS8" s="4" t="s">
+      <c r="AS8" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="AT8" s="4" t="s">
+      <c r="AT8" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AU8" s="5" t="s">
+      <c r="AU8" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="AV8" s="4" t="s">
+      <c r="AV8" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="AW8" s="4" t="s">
+      <c r="AW8" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AX8" s="7" t="s">
+      <c r="AX8" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="AY8" s="8" t="s">
+      <c r="AY8" s="12" t="s">
         <v>39</v>
       </c>
       <c r="AZ8" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="BA8" s="4" t="s">
+      <c r="BA8" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="BB8" s="4" t="s">
+      <c r="BB8" s="7" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" spans="1:54" x14ac:dyDescent="0.3">
-      <c r="A9" s="1" t="s">
+      <c r="A9" s="5" t="s">
         <v>36</v>
       </c>
     </row>

</xml_diff>